<commit_message>
Schedule Python Project 26/04/2022 Update
</commit_message>
<xml_diff>
--- a/prototype.xlsx
+++ b/prototype.xlsx
@@ -150,37 +150,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF7E591A"/>
+        <fgColor rgb="FF08E5B7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF8D43A1"/>
+        <fgColor rgb="FF01FD75"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE79A81"/>
+        <fgColor rgb="FFA06CBA"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF94540"/>
+        <fgColor rgb="FF75449F"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF4D4B4E"/>
+        <fgColor rgb="FF0BB5DC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCD0901"/>
+        <fgColor rgb="FF2BC818"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>

</xml_diff>